<commit_message>
walmart scrape and image transform
</commit_message>
<xml_diff>
--- a/walmart_products_withprice.xlsx
+++ b/walmart_products_withprice.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,136 +452,146 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>361630632749</v>
+        <v>7846238951</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails French Twist Non Damaging Easy to Apply 1.0000 EA - 0361630632749</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
+          <t>Salon Perfect Artificial Press On Nails 156 Modern French Deep White 1.0000 EA - 0007846238951</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>$5.94</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>361630632748</v>
+        <v>7846238954</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails Onyx Pected Non Damaging Easy to Apply 1.0000 EA - 0361630632748</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
+          <t>Salon Perfect Artificial Press On Nails 215 Modern Nostalgia Blue Green UFO 1.0000 EA - 0007846238954</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$6.94</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>361630632757</v>
+        <v>7846238960</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails Rocket Fuel Non Damaging Easy to Apply 1.0000 EA - 0361630632757</t>
+          <t>Salon Perfect Artificial Press On Nails 168 Pearl Flower 1.0000 EA - 0007846238960</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$7.48</t>
+          <t>$7.94</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>361630632752</v>
+        <v>7846239400</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails Affairy to Remember Non Damaging Easy to Apply 1.0000 EA - 0361630632752</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
+          <t>Salon Perfect Artificial Fake Press ons 381 Glass Magenta Medium Almond File and Glue Included 30 Nails 1.0000 EA - 0007846239400</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$7.94</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>361630632736</v>
+        <v>7846236763</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails Sunshine Spritz Non Damaging Easy to Apply 1.0000 EA - 0361630632736</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
+          <t>Salon Perfect Artificial Fake Press Ons 255 Glazed Peach French Tip Short Round Squoval File and Glue Included 30 Nails 1.0000 EA - 0007846236763</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$6.94</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7846238561</v>
+        <v>7846238345</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Salon Perfect Nail Art Sticker Kit Celestial Charms 1 Sheet 1.0000 EA - 0007846238561</t>
+          <t>Salon Perfect Artificial Fake Press Ons 337 Modern Nostalgia Smiley Checkered Short Almond File and Glue Included 30 Nails 1.0000 EA - 0007846238345</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$3.98</t>
+          <t>$6.94</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>361630632730</v>
+        <v>7846238354</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails I Heart You Non Damaging Easy to Apply 1.0000 EA - 0361630632730</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
+          <t>Salon Perfect Artificial Fake Press On Nails 346 Viral Nail Edit Lemon Medium Almond File and Glue Included 30 Nails 1.0000 EA - 0007846238354</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$9.98</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>81016355305</v>
+        <v>7846238961</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Maximalist Short Round Press On Nails Sky Chrome 42 Pieces 42.0000 EA - 0081016355305</t>
+          <t>Salon Perfect Artificial Press On Nails 170 Pearl French 1.0000 EA - 0007846238961</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>$9.98</t>
+          <t>$7.94</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7846238955</v>
+        <v>7846238445</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Salon Perfect Artificial Press On Nails 195 Aura Jelly Blue Purple 1.0000 EA - 0007846238955</t>
+          <t>Salon Perfect Artificial Press On Nails 308 Viral Nail Edit Gold Cosmic 1.0000 EA - 0007846238445</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$6.94</t>
+          <t>$9.98</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>81011624813</v>
+        <v>81011624835</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Olive June Super Stick Mani Oval Medium Press On Tabs Dainty Bows 32 Pieces 1.0000 EA - 0081011624813</t>
+          <t>Olive June Ultra Strong Nail Glue 1.0000 EA - 0081011624835</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -592,144 +602,142 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>81011624842</v>
+        <v>7846239402</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Olive June Super Stick Mani Oval Medium Press On Tabs Pink Chrome Ombre 32 Pieces 1.0000 EA - 0081011624842</t>
+          <t>Salon Perfect Artificial Fake Press ons 383 Glass Light Pink Short Almond File and Glue Included 30 Nails 1.0000 EA - 0007846239402</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$8.98</t>
+          <t>$7.94</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>7846238357</v>
+        <v>7846239401</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Salon Perfect Artificial Fake Press ons 349 Viral Nail Edit Snake Medium Almond File and Glue Included 30 Nails 1.0000 EA - 0007846238357</t>
+          <t>Salon Perfect Artificial Fake Press Ons 382 Glass Violet Short Almond File and Glue Included 30 Nails 1.0000 EA - 0007846239401</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$9.98</t>
+          <t>$7.94</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>7846238347</v>
+        <v>7846238447</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Salon Perfect Artificial Fake Press Ons 339 Modern Nostalgia Western Cowboy Medium Almond File and Glue Included 30 Nails 1.0000 EA - 0007846238347</t>
+          <t>Salon Perfect Artificial Press On Nails 310 Viral Naid Edit Magnetic Heart 1.0000 EA - 0007846238447</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>$6.94</t>
+          <t>$9.98</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>7846238348</v>
+        <v>7846238952</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Salon Perfect Artificial Fake Press Ons 340 Modern Nostalgia Ying Yang Medium Almond File and Glue Included 30 Nails 1.0000 EA - 0007846238348</t>
+          <t>Salon Perfect Artificial Press on Nails 178 Modern French White Ombre 1.0000 EA - 0007846238952</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$6.94</t>
+          <t>$5.94</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>361630632756</v>
+        <v>81011624628</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails Lost In The Frost Non Damaging Easy to Apply 1.0000 EA - 0361630632756</t>
+          <t>Olive June Instant Mani Maximalist Medium Stiletto Press On Nails Sharp French 42 Pieces 1.0000 EA - 0081011624628</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$7.48</t>
+          <t>$9.98</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>361630632735</v>
+        <v>7846238360</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails Swoop There It Is Non Damaging Easy to Apply 1.0000 EA - 0361630632735</t>
+          <t>Salon Perfect Artificial Fake Press Ons 352 Viral Nail Edit Pink Shell Short Almond File and Glue Included 30 Nails 1.0000 EA - 0007846238360</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>$7.48</t>
+          <t>$9.98</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>81011624972</v>
+        <v>361630632749</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Medium Almond Press On Nails Sage Velvet 42 Pieces 1.0000 EA - 0081011624972</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>$9.98</t>
-        </is>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails French Twist Non Damaging Easy to Apply 1.0000 EA - 0361630632749</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>361630632732</v>
+        <v>361630632748</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails Asap Apple Non Damaging Easy to Apply 1.0000 EA - 0361630632732</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>$7.48</t>
-        </is>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails Onyx Pected Non Damaging Easy to Apply 1.0000 EA - 0361630632748</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>361630632746</v>
+        <v>361630632757</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails Soul Pink Non Damaging Easy to Apply 1.0000 EA - 0361630632746</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails Rocket Fuel Non Damaging Easy to Apply 1.0000 EA - 0361630632757</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$7.48</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>361630632740</v>
+        <v>361630632752</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails A La Mode Non Damaging Easy to Apply 1.0000 EA - 0361630632740</t>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails Affairy to Remember Non Damaging Easy to Apply 1.0000 EA - 0361630632752</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -738,11 +746,11 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>361630632747</v>
+        <v>361630632736</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails Hyp Nautical Non Damaging Easy to Apply 1.0000 EA - 0361630632747</t>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails Sunshine Spritz Non Damaging Easy to Apply 1.0000 EA - 0361630632736</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -751,874 +759,872 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>7846237080</v>
+        <v>7846238561</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Salon Perfect Artificial Fake Press On Tips 307 Gel X Tension Clear Medium Almond 120 Nails 1.0000 EA - 0007846237080</t>
+          <t>Salon Perfect Nail Art Sticker Kit Celestial Charms 1 Sheet 1.0000 EA - 0007846238561</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>$9.98</t>
+          <t>$3.98</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>7846238448</v>
+        <v>361630632730</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Salon Perfect Artificial Fake Press on Tips 302 Gel X Tension Clear Medium Coffin 120 Nails 1.0000 EA - 0007846238448</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>$9.98</t>
-        </is>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails I Heart You Non Damaging Easy to Apply 1.0000 EA - 0361630632730</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>406466525171</v>
+        <v>81016355305</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>OPI On Point Instant Press On Mani Hue cid Dreams 1.0000 EA - 0406466525171</t>
+          <t>Olive June Instant Mani Maximalist Short Round Press On Nails Sky Chrome 42 Pieces 42.0000 EA - 0081016355305</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>$10.98</t>
+          <t>$9.98</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>81011624687</v>
+        <v>7846238955</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Short Round Press On Nails Silver Foil Stars 42 Pieces 1.0000 EA - 0081011624687</t>
+          <t>Salon Perfect Artificial Press On Nails 195 Aura Jelly Blue Purple 1.0000 EA - 0007846238955</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>$9.98</t>
+          <t>$6.94</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>85004456509</v>
+        <v>81011624813</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PaintLab Reusable Gel Press on Nails Kit Coffin Shape Purple Lavender Butterfly 30 Count 30.0000 EA - 0085004456509</t>
+          <t>Olive June Super Stick Mani Oval Medium Press On Tabs Dainty Bows 32 Pieces 1.0000 EA - 0081011624813</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>$9.97</t>
+          <t>$7.98</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>7846238449</v>
+        <v>81011624842</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Salon Perfect Artificial Press On Nails 305 Gel X Tension Clear Stilletto 1.0000 EA - 0007846238449</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>0</v>
+          <t>Olive June Super Stick Mani Oval Medium Press On Tabs Pink Chrome Ombre 32 Pieces 1.0000 EA - 0081011624842</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$8.98</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>7846238661</v>
+        <v>7846238357</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Salon Perfect Gel Nail Polish Remover Kit Includes Foil Pusher and File Use with Acetone 50 Foils 1.0000 EA - 0007846238661</t>
+          <t>Salon Perfect Artificial Fake Press ons 349 Viral Nail Edit Snake Medium Almond File and Glue Included 30 Nails 1.0000 EA - 0007846238357</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>$6.98</t>
+          <t>$9.98</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>81011624653</v>
+        <v>7846238347</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Minimalist Short Almond Press On Nails Blush Syrup Gradient 42 Pieces 1.0000 EA - 0081011624653</t>
+          <t>Salon Perfect Artificial Fake Press Ons 339 Modern Nostalgia Western Cowboy Medium Almond File and Glue Included 30 Nails 1.0000 EA - 0007846238347</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>$9.98</t>
+          <t>$6.94</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>81011624650</v>
+        <v>7846238348</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Press On Nails Cdj Syrup Gradient 1.0000 EA - 0081011624650</t>
+          <t>Salon Perfect Artificial Fake Press Ons 340 Modern Nostalgia Ying Yang Medium Almond File and Glue Included 30 Nails 1.0000 EA - 0007846238348</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>$9.98</t>
+          <t>$6.94</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>81011624844</v>
+        <v>361630632756</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Olive June Super Stick Mani Oval Medium Press On Tabs Plaza Shimmer 32 Pieces 1.0000 EA - 0081011624844</t>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails Lost In The Frost Non Damaging Easy to Apply 1.0000 EA - 0361630632756</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>$10.63</t>
+          <t>$7.48</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>7846237059</v>
+        <v>361630632735</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Salon Perfect Artificial Press on Nails 306 Gel X Tension French Square 1.0000 EA - 0007846237059</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>0</v>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails Swoop There It Is Non Damaging Easy to Apply 1.0000 EA - 0361630632735</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>$7.48</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>7846237105</v>
+        <v>81011624972</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Salon Perfect Artificial Press on Nails 304 Gel X Tension French Almond 1.0000 EA - 0007846237105</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>0</v>
+          <t>Olive June Instant Mani Medium Almond Press On Nails Sage Velvet 42 Pieces 1.0000 EA - 0081011624972</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>$9.98</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>85004456510</v>
+        <v>361630632732</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>PaintLab Reusable Gel Press on Nails Kit Almond Shape Cherry Bomb 30 Count 30.0000 EA - 0085004456510</t>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails Asap Apple Non Damaging Easy to Apply 1.0000 EA - 0361630632732</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>$9.97</t>
+          <t>$7.48</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>85002955452</v>
+        <v>361630632746</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>PaintLab Reusable Gel Press on Nails Kit Almond Shape Strawberry Pink 30 Count 30.0000 EA - 0085002955452</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>$9.97</t>
-        </is>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails Soul Pink Non Damaging Easy to Apply 1.0000 EA - 0361630632746</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>85004871702</v>
+        <v>361630632740</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>PaintLab Reusable Gel Press on Nails Kit Almond Shape Aura 888 Blue 30 Count 30.0000 EA - 0085004871702</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>$15.99</t>
-        </is>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails A La Mode Non Damaging Easy to Apply 1.0000 EA - 0361630632740</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>81011624843</v>
+        <v>361630632747</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Olive June Super Stick Mani Oval Medium Press On Tabs BP Velvet 32 Pieces 1.0000 EA - 0081011624843</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>$10.34</t>
-        </is>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails Hyp Nautical Non Damaging Easy to Apply 1.0000 EA - 0361630632747</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>81011624819</v>
+        <v>7846237080</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>OLIVE JUNE PRESS ON TABS DAISY POP 1.0000 EA - 0081011624819</t>
+          <t>Salon Perfect Artificial Fake Press On Tips 307 Gel X Tension Clear Medium Almond 120 Nails 1.0000 EA - 0007846237080</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>$7.98</t>
+          <t>$9.98</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>81011624585</v>
+        <v>7846238448</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Olive June Super Stick Mani Round Short Press On Tabs Red Lollipop 32 Pieces 1.0000 EA - 0081011624585</t>
+          <t>Salon Perfect Artificial Fake Press on Tips 302 Gel X Tension Clear Medium Coffin 120 Nails 1.0000 EA - 0007846238448</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>$8.33</t>
+          <t>$9.98</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>81011624859</v>
+        <v>406466525171</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Press On Nails HZ Velvet 42 Pieces 1.0000 EA - 0081011624859</t>
+          <t>OPI On Point Instant Press On Mani Hue cid Dreams 1.0000 EA - 0406466525171</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>$9.98</t>
+          <t>$10.98</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>361630632743</v>
+        <v>81011624687</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Perfect Press On Nails Light Years Non Damaging Easy to Apply 1.0000 EA - 0361630632743</t>
+          <t>Olive June Instant Mani Short Round Press On Nails Silver Foil Stars 42 Pieces 1.0000 EA - 0081011624687</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>$7.48</t>
+          <t>$9.98</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>361630513422</v>
+        <v>85004456509</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Nail Accents Bubbly Pearls 1.0000 EA - 0361630513422</t>
+          <t>PaintLab Reusable Gel Press on Nails Kit Coffin Shape Purple Lavender Butterfly 30 Count 30.0000 EA - 0085004456509</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>$10.01</t>
+          <t>$9.97</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>81011624471</v>
+        <v>7846238449</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Olive June Super Stick Mani Squoval Short Press On Tabs Simple Squiggle 32 Pieces 1.0000 EA - 0081011624471</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>$9.53</t>
-        </is>
+          <t>Salon Perfect Artificial Press On Nails 305 Gel X Tension Clear Stilletto 1.0000 EA - 0007846238449</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>81011624126</v>
+        <v>7846238661</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Round Short Press On Nails Pink Pen Pal Jelly 42 Pieces 1.0000 EA - 0081011624126</t>
+          <t>Salon Perfect Gel Nail Polish Remover Kit Includes Foil Pusher and File Use with Acetone 50 Foils 1.0000 EA - 0007846238661</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>$13.49</t>
+          <t>$6.98</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>361630520009</v>
+        <v>81011624653</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Nail Accents Glam Geometric 1.0000 EA - 0361630520009</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>0</v>
+          <t>Olive June Instant Mani Minimalist Short Almond Press On Nails Blush Syrup Gradient 42 Pieces 1.0000 EA - 0081011624653</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>$9.98</t>
+        </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>361630513420</v>
+        <v>81011624650</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Sally Hansen Salon Effects Nail Accents Wild Side 1.0000 EA - 0361630513420</t>
-        </is>
-      </c>
-      <c r="C47" t="n">
-        <v>0</v>
+          <t>Olive June Instant Mani Press On Nails Cdj Syrup Gradient 1.0000 EA - 0081011624650</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>$9.98</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>81895702871</v>
+        <v>81011624844</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Extra Short Round Press On Nails Pink Baby Starfish 42 Pieces 1.0000 EA - 0081895702871</t>
+          <t>Olive June Super Stick Mani Oval Medium Press On Tabs Plaza Shimmer 32 Pieces 1.0000 EA - 0081011624844</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>$10.00</t>
+          <t>$10.63</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>81011624814</v>
+        <v>7846237059</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Olive June Super Stick Mani Round Extra Short Press On Tabs Blue Midnight Mixed 32 Pieces 1.0000 EA - 0081011624814</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>$6.97</t>
-        </is>
+          <t>Salon Perfect Artificial Press on Nails 306 Gel X Tension French Square 1.0000 EA - 0007846237059</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>81011624469</v>
+        <v>7846237105</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Olive June Super Stick Mani Squoval Short Press On Tabs Vintage 32 Pieces 1.0000 EA - 0081011624469</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>$9.66</t>
-        </is>
+          <t>Salon Perfect Artificial Press on Nails 304 Gel X Tension French Almond 1.0000 EA - 0007846237105</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>81011624132</v>
+        <v>85004456510</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Almond Long Press On Nails Sheer Pink CCT 42 Pieces 1.0000 EA - 0081011624132</t>
+          <t>PaintLab Reusable Gel Press on Nails Kit Almond Shape Cherry Bomb 30 Count 30.0000 EA - 0085004456510</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>$10.75</t>
+          <t>$9.97</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>81011624141</v>
+        <v>85002955452</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Round Short Press On Nails Green Besties 42 Pieces 1.0000 EA - 0081011624141</t>
+          <t>PaintLab Reusable Gel Press on Nails Kit Almond Shape Strawberry Pink 30 Count 30.0000 EA - 0085002955452</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>$9.25</t>
+          <t>$9.97</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>81011624845</v>
+        <v>85004871702</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>OLIVE JUNE PRESS ON TABS EFFECTS GLAZED FRENCH 1.0000 EA - 0081011624845</t>
-        </is>
-      </c>
-      <c r="C53" t="n">
-        <v>0</v>
+          <t>PaintLab Reusable Gel Press on Nails Kit Almond Shape Aura 888 Blue 30 Count 30.0000 EA - 0085004871702</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>$15.99</t>
+        </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>81011624051</v>
+        <v>81011624843</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Olive June Press on Artificial Nails Almond Medium Social Studies Blue 42 Ct 42.0000 EA - 0081011624051</t>
+          <t>Olive June Super Stick Mani Oval Medium Press On Tabs BP Velvet 32 Pieces 1.0000 EA - 0081011624843</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>$11.02</t>
+          <t>$10.34</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>81895702852</v>
+        <v>81011624819</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Olive June Press on Squoval XS False Nails CV Red 42 Count 1.0000 EA - 0081895702852</t>
+          <t>OLIVE JUNE PRESS ON TABS DAISY POP 1.0000 EA - 0081011624819</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>$13.49</t>
+          <t>$7.98</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>81011624127</v>
+        <v>81011624585</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Olive June Instant Mani Short Round Press on Nails Pink Chrome French 42 Pieces 1.0000 EA - 0081011624127</t>
+          <t>Olive June Super Stick Mani Round Short Press On Tabs Red Lollipop 32 Pieces 1.0000 EA - 0081011624585</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>$13.49</t>
+          <t>$8.33</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>73150991962</v>
+        <v>81011624859</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>KISS Classy Press On Nails Players White Short Oval 28 Count 28.0000 EA - 0073150991962</t>
+          <t>Olive June Instant Mani Press On Nails HZ Velvet 42 Pieces 1.0000 EA - 0081011624859</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>$5.97</t>
+          <t>$9.98</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>73150991586</v>
+        <v>361630632743</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>KISS Salon X tend Press on Nails Perk Beige Medium Coffin 30 Count 30.0000 EA - 0073150991586</t>
+          <t>Sally Hansen Salon Effects Perfect Press On Nails Light Years Non Damaging Easy to Apply 1.0000 EA - 0361630632743</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>$19.97</t>
+          <t>$7.48</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>73150980017</v>
+        <v>361630513422</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>KISS Glue Off Press on Nail Remover 1.0000 EA - 0073150980017</t>
-        </is>
-      </c>
-      <c r="C59" t="n">
-        <v>0</v>
+          <t>Sally Hansen Salon Effects Nail Accents Bubbly Pearls 1.0000 EA - 0361630513422</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>$10.01</t>
+        </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>73150993388</v>
+        <v>81011624471</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color FX Press on Nails Sour Love Silver Short Oval 30 Count 30.0000 EA - 0073150993388</t>
-        </is>
-      </c>
-      <c r="C60" t="n">
-        <v>0</v>
+          <t>Olive June Super Stick Mani Squoval Short Press On Tabs Simple Squiggle 32 Pieces 1.0000 EA - 0081011624471</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>$9.53</t>
+        </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>73150993790</v>
+        <v>81011624126</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color FX Press on Nails Starry Pink Short Oval 30 Count 30.0000 EA - 0073150993790</t>
+          <t>Olive June Instant Mani Round Short Press On Nails Pink Pen Pal Jelly 42 Pieces 1.0000 EA - 0081011624126</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>$10.99</t>
+          <t>$13.49</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>73150991404</v>
+        <v>361630520009</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color FX Press on Nails Starstruck Beige Short Squoval 30 Count 1.0000 EA - 0073150991404</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>$10.99</t>
-        </is>
+          <t>Sally Hansen Salon Effects Nail Accents Glam Geometric 1.0000 EA - 0361630520009</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>73150991405</v>
+        <v>361630513420</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color FX Press on Nails After Hours Green Short Squoval 30 Count 1.0000 EA - 0073150991405</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>$8.97</t>
-        </is>
+          <t>Sally Hansen Salon Effects Nail Accents Wild Side 1.0000 EA - 0361630513420</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>73150995469</v>
+        <v>81895702871</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>KISS Gel Fantasy Magnetic Press On Nails Solid Red Medium Oval 28 Count 28.0000 EA - 0073150995469</t>
+          <t>Olive June Instant Mani Extra Short Round Press On Nails Pink Baby Starfish 42 Pieces 1.0000 EA - 0081895702871</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>$9.99</t>
+          <t>$10.00</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>73150991379</v>
+        <v>81011624814</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>KISS imPRESS Press on Nails Portal Purple Medium Coffin 30 Count 30.0000 EA - 0073150991379</t>
+          <t>Olive June Super Stick Mani Round Extra Short Press On Tabs Blue Midnight Mixed 32 Pieces 1.0000 EA - 0081011624814</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>$10.97</t>
+          <t>$6.97</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>73150993385</v>
+        <v>81011624469</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color FX Press on Nails Walk Out Pink Short Oval 30 Count 1.0000 EA - 0073150993385</t>
+          <t>Olive June Super Stick Mani Squoval Short Press On Tabs Vintage 32 Pieces 1.0000 EA - 0081011624469</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>$8.97</t>
+          <t>$9.66</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>73150986734</v>
+        <v>81011624132</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color Medium Coffin Press On Nails Frosting 30 Count 1.0000 EA - 0073150986734</t>
-        </is>
-      </c>
-      <c r="C67" t="n">
-        <v>0</v>
+          <t>Olive June Instant Mani Almond Long Press On Nails Sheer Pink CCT 42 Pieces 1.0000 EA - 0081011624132</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>$10.75</t>
+        </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>73150993788</v>
+        <v>81011624141</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color FX Press on Nails Reconnect Blue Short Oval 30 Count 30.0000 EA - 0073150993788</t>
+          <t>Olive June Instant Mani Round Short Press On Nails Green Besties 42 Pieces 1.0000 EA - 0081011624141</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>$8.97</t>
+          <t>$9.25</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>73150993386</v>
+        <v>81011624845</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color FX Press on Nails Fly Up Silver Short Oval 30 Count 1.0000 EA - 0073150993386</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>$8.97</t>
-        </is>
+          <t>OLIVE JUNE PRESS ON TABS EFFECTS GLAZED FRENCH 1.0000 EA - 0081011624845</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>73150991550</v>
+        <v>81011624051</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color FX Press on Nails Dimension Neutral Short Squoval 30 Count 1.0000 EA - 0073150991550</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr"/>
+          <t>Olive June Press on Artificial Nails Almond Medium Social Studies Blue 42 Ct 42.0000 EA - 0081011624051</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>$11.02</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>73150995934</v>
+        <v>81895702852</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>KISS Voguish Fantasy Press on Nails Luminary Pink Short Oval 28 Count 28.0000 EA - 0073150995934</t>
+          <t>Olive June Press on Squoval XS False Nails CV Red 42 Count 1.0000 EA - 0081895702852</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>$7.97</t>
+          <t>$13.49</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>73150995933</v>
+        <v>81011624127</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>KISS Gel Fantasy Sculpted Press on Nails Sweater Weather Beige Medium Almond 28 Count 28.0000 EA - 0073150995933</t>
+          <t>Olive June Instant Mani Short Round Press on Nails Pink Chrome French 42 Pieces 1.0000 EA - 0081011624127</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>$7.97</t>
+          <t>$13.49</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>73150921398</v>
+        <v>73150991962</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>KISS Voguish Fantasy Press On Nails Golden Warmth White Medium Oval 28 Count 28.0000 EA - 0073150921398</t>
+          <t>KISS Classy Press On Nails Players White Short Oval 28 Count 28.0000 EA - 0073150991962</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>$7.97</t>
+          <t>$5.97</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>73150993381</v>
+        <v>73150991586</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>KISS imPRESS Design Press on Nails Wild Venus Pink Medium Almond 30 Count 1.0000 EA - 0073150993381</t>
+          <t>KISS Salon X tend Press on Nails Perk Beige Medium Coffin 30 Count 30.0000 EA - 0073150991586</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>$7.97</t>
+          <t>$19.97</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>73150994332</v>
+        <v>73150980017</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>KISS imPRESS Press on Nails Velvet Twilight Beige Short Oval 30 Count 1.0000 EA - 0073150994332</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>$6.27</t>
-        </is>
+          <t>KISS Glue Off Press on Nail Remover 1.0000 EA - 0073150980017</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>73150921227</v>
+        <v>73150993388</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>KISS Gel Fantasy Allure Press on Nails Fancy You Dearly Pink Short Oval 30 Count 30.0000 EA - 0073150921227</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>$10.97</t>
-        </is>
+          <t>KISS imPRESS Color FX Press on Nails Sour Love Silver Short Oval 30 Count 30.0000 EA - 0073150993388</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>73150921505</v>
+        <v>73150993790</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>KISS Classy Premium Press on Nails Croissant City White Medium Almond 30 Count 30.0000 EA - 0073150921505</t>
+          <t>KISS imPRESS Color FX Press on Nails Starry Pink Short Oval 30 Count 30.0000 EA - 0073150993790</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>$8.97</t>
+          <t>$10.99</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>73150993383</v>
+        <v>73150991404</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>KISS imPRESS Design Press on Nails Utopian Multicolor Medium Almond 30 Count 30.0000 EA - 0073150993383</t>
+          <t>KISS imPRESS Color FX Press on Nails Starstruck Beige Short Squoval 30 Count 1.0000 EA - 0073150991404</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>$7.97</t>
+          <t>$10.99</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>73150995456</v>
+        <v>73150991405</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>KISS Gel Fantasy Allure Press on Nails Glide Pink Medium Almond 30 Count 30.0000 EA - 0073150995456</t>
+          <t>KISS imPRESS Color FX Press on Nails After Hours Green Short Squoval 30 Count 1.0000 EA - 0073150991405</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>$10.97</t>
+          <t>$8.97</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>73150921299</v>
+        <v>73150995469</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>KISS imPRESS Press on Toenails Design Blanc Chic Beige Short Squoval 24 Count 24.0000 EA - 0073150921299</t>
+          <t>KISS Gel Fantasy Magnetic Press On Nails Solid Red Medium Oval 28 Count 28.0000 EA - 0073150995469</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>$7.97</t>
+          <t>$9.99</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>73150994701</v>
+        <v>73150991379</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>KISS imPRESS Design Press on Nails Secretly Yours Pink Short Oval 30 Count 30.0000 EA - 0073150994701</t>
+          <t>KISS imPRESS Press on Nails Portal Purple Medium Coffin 30 Count 30.0000 EA - 0073150991379</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>$7.97</t>
+          <t>$10.97</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>73150993389</v>
+        <v>73150993385</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color FX Press on Nails Around You Pink Short Oval 30 Count 30.0000 EA - 0073150993389</t>
+          <t>KISS imPRESS Color FX Press on Nails Walk Out Pink Short Oval 30 Count 1.0000 EA - 0073150993385</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1629,71 +1635,65 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>73150921228</v>
+        <v>73150986734</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>KISS Gel Fantasy Allure Press on Nails Sunday Breeze Blue Short Almond 30 Count 30.0000 EA - 0073150921228</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>$10.97</t>
-        </is>
+          <t>KISS imPRESS Color Medium Coffin Press On Nails Frosting 30 Count 1.0000 EA - 0073150986734</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>73150994715</v>
+        <v>73150993788</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color Press on Nails All Smiles Pink Short Squoval 30 Count 30.0000 EA - 0073150994715</t>
+          <t>KISS imPRESS Color FX Press on Nails Reconnect Blue Short Oval 30 Count 30.0000 EA - 0073150993788</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>$6.27</t>
+          <t>$8.97</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>73150921236</v>
+        <v>73150993386</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>KISS Salon Design Press on Nails Dazzling Muse Green Short Squoval 24 Count 28.0000 EA - 0073150921236</t>
+          <t>KISS imPRESS Color FX Press on Nails Fly Up Silver Short Oval 30 Count 1.0000 EA - 0073150993386</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>$5.97</t>
+          <t>$8.97</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>73150921234</v>
+        <v>73150991550</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>KISS Salon Color Press on Nails Truthful Red Short Squoval 28 Count 28.0000 EA - 0073150921234</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>$5.97</t>
-        </is>
-      </c>
+          <t>KISS imPRESS Color FX Press on Nails Dimension Neutral Short Squoval 30 Count 1.0000 EA - 0073150991550</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>73150921231</v>
+        <v>73150995934</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>KISS Gel Fantasy Magnetic Press On Nails Velvet Spark Purple Short Oval 28 Count 28.0000 EA - 0073150921231</t>
+          <t>KISS Voguish Fantasy Press on Nails Luminary Pink Short Oval 28 Count 28.0000 EA - 0073150995934</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -1704,146 +1704,146 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>73150921229</v>
+        <v>73150995933</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>KISS Gel Fantasy Allure Press on Nails Gentle Whisper Yellow Long Square 30 Count 30.0000 EA - 0073150921229</t>
+          <t>KISS Gel Fantasy Sculpted Press on Nails Sweater Weather Beige Medium Almond 28 Count 28.0000 EA - 0073150995933</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>$11.99</t>
+          <t>$7.97</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>73150921237</v>
+        <v>73150921398</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>KISS Salon Design Press on Nails Boldly Glitzy Red Short Coffin 24 Count 28.0000 EA - 0073150921237</t>
+          <t>KISS Voguish Fantasy Press On Nails Golden Warmth White Medium Oval 28 Count 28.0000 EA - 0073150921398</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>$5.97</t>
+          <t>$7.97</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>73150993425</v>
+        <v>73150993381</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>KISS Gel Fantasy Allure Press On Nails Change Chance Silver Short Oval 28 Count 28.0000 EA - 0073150993425</t>
+          <t>KISS imPRESS Design Press on Nails Wild Venus Pink Medium Almond 30 Count 1.0000 EA - 0073150993381</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>$10.97</t>
+          <t>$7.97</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>73150994730</v>
+        <v>73150994332</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>KISS imPRESS Press On Nails Design Dazzle White Medium Almond 30 Count 30.0000 EA - 0073150994730</t>
+          <t>KISS imPRESS Press on Nails Velvet Twilight Beige Short Oval 30 Count 1.0000 EA - 0073150994332</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>$7.97</t>
+          <t>$6.27</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>73150994716</v>
+        <v>73150921227</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color Press on Nails Prime Time Orange Short Squoval 30 Count 30.0000 EA - 0073150994716</t>
+          <t>KISS Gel Fantasy Allure Press on Nails Fancy You Dearly Pink Short Oval 30 Count 30.0000 EA - 0073150921227</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>$7.99</t>
+          <t>$10.97</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>73150921129</v>
+        <v>73150921505</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>KISS imPRESS Press on Toenails Color Angel Vibes White Short Squoval 24 Count 24.0000 EA - 0073150921129</t>
+          <t>KISS Classy Premium Press on Nails Croissant City White Medium Almond 30 Count 30.0000 EA - 0073150921505</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>$6.27</t>
+          <t>$8.97</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>73150994717</v>
+        <v>73150993383</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color Press on Nails Quench It Blue Short Squoval 30 Count 30.0000 EA - 0073150994717</t>
+          <t>KISS imPRESS Design Press on Nails Utopian Multicolor Medium Almond 30 Count 30.0000 EA - 0073150993383</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>$6.27</t>
+          <t>$7.97</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>73150921232</v>
+        <v>73150995456</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>KISS Salon Color Press on Nails Afternoon Tea Pink Real Short Oval 28 Count 28.0000 EA - 0073150921232</t>
+          <t>KISS Gel Fantasy Allure Press on Nails Glide Pink Medium Almond 30 Count 30.0000 EA - 0073150995456</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>$5.97</t>
+          <t>$10.97</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>73150994718</v>
+        <v>73150921299</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color Press on Nails The Answer Purple Short Oval 30 Count 30.0000 EA - 0073150994718</t>
+          <t>KISS imPRESS Press on Toenails Design Blanc Chic Beige Short Squoval 24 Count 24.0000 EA - 0073150921299</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>$6.27</t>
+          <t>$7.97</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>73150994729</v>
+        <v>73150994701</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>KISS imPRESS Press on Nails Like A Star Black Medium Coffin 30 Count 30.0000 EA - 0073150994729</t>
+          <t>KISS imPRESS Design Press on Nails Secretly Yours Pink Short Oval 30 Count 30.0000 EA - 0073150994701</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -1854,11 +1854,11 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>73150991406</v>
+        <v>73150993389</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>KISS imPRESS Color FX Press on Nails Meta Blue Short Squoval 30 Count 1.0000 EA - 0073150991406</t>
+          <t>KISS imPRESS Color FX Press on Nails Around You Pink Short Oval 30 Count 30.0000 EA - 0073150993389</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -1869,44 +1869,284 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>73150991897</v>
+        <v>73150921228</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>KISS Gel Fantasy Allure Press On Nails Hottiest Thing White Short Coffin 28 Count 1.0000 EA - 0073150991897</t>
+          <t>KISS Gel Fantasy Allure Press on Nails Sunday Breeze Blue Short Almond 30 Count 30.0000 EA - 0073150921228</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>$11.99</t>
+          <t>$10.97</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>73150993355</v>
+        <v>73150994715</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>KISS imPRESS Press on Nails Slip Dress Beige Short Oval 30 Count 1.0000 EA - 0073150993355</t>
+          <t>KISS imPRESS Color Press on Nails All Smiles Pink Short Squoval 30 Count 30.0000 EA - 0073150994715</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>$8.54</t>
+          <t>$6.27</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
+        <v>73150921236</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>KISS Salon Design Press on Nails Dazzling Muse Green Short Squoval 24 Count 28.0000 EA - 0073150921236</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>$5.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>73150921234</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>KISS Salon Color Press on Nails Truthful Red Short Squoval 28 Count 28.0000 EA - 0073150921234</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>$5.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>73150921231</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>KISS Gel Fantasy Magnetic Press On Nails Velvet Spark Purple Short Oval 28 Count 28.0000 EA - 0073150921231</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>$7.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>73150921229</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>KISS Gel Fantasy Allure Press on Nails Gentle Whisper Yellow Long Square 30 Count 30.0000 EA - 0073150921229</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>$11.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>73150921237</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>KISS Salon Design Press on Nails Boldly Glitzy Red Short Coffin 24 Count 28.0000 EA - 0073150921237</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>$5.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>73150993425</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>KISS Gel Fantasy Allure Press On Nails Change Chance Silver Short Oval 28 Count 28.0000 EA - 0073150993425</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>$10.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>73150994730</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>KISS imPRESS Press On Nails Design Dazzle White Medium Almond 30 Count 30.0000 EA - 0073150994730</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>$7.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>73150994716</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>KISS imPRESS Color Press on Nails Prime Time Orange Short Squoval 30 Count 30.0000 EA - 0073150994716</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>$7.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>73150921129</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>KISS imPRESS Press on Toenails Color Angel Vibes White Short Squoval 24 Count 24.0000 EA - 0073150921129</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>$6.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>73150994717</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>KISS imPRESS Color Press on Nails Quench It Blue Short Squoval 30 Count 30.0000 EA - 0073150994717</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>$6.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>73150921232</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>KISS Salon Color Press on Nails Afternoon Tea Pink Real Short Oval 28 Count 28.0000 EA - 0073150921232</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>$5.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>73150994718</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>KISS imPRESS Color Press on Nails The Answer Purple Short Oval 30 Count 30.0000 EA - 0073150994718</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>$6.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>73150994729</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>KISS imPRESS Press on Nails Like A Star Black Medium Coffin 30 Count 30.0000 EA - 0073150994729</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>$7.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>73150991406</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>KISS imPRESS Color FX Press on Nails Meta Blue Short Squoval 30 Count 1.0000 EA - 0073150991406</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>$8.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>73150991897</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>KISS Gel Fantasy Allure Press On Nails Hottiest Thing White Short Coffin 28 Count 1.0000 EA - 0073150991897</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>$11.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>73150993355</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>KISS imPRESS Press on Nails Slip Dress Beige Short Oval 30 Count 1.0000 EA - 0073150993355</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>$8.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
         <v>73150993789</v>
       </c>
-      <c r="B101" t="inlineStr">
+      <c r="B117" t="inlineStr">
         <is>
           <t>KISS imPRESS Color FX Press on Nails Floating Pink Short Oval 30 Count 30.0000 EA - 0073150993789</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
+      <c r="C117" t="inlineStr">
         <is>
           <t>$10.99</t>
         </is>

</xml_diff>